<commit_message>
Change font of commands.
</commit_message>
<xml_diff>
--- a/excel/base/ExcelCheatsheet.xlsx
+++ b/excel/base/ExcelCheatsheet.xlsx
@@ -209,14 +209,14 @@
     <t>????????</t>
   </si>
   <si>
-    <t>v0.1.1</t>
+    <t>v0.1.2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -247,13 +247,6 @@
       <name val="Helvetica Light"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color theme="1"/>
-      <name val="Source Han Code JP R"/>
-      <charset val="128"/>
-    </font>
-    <font>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Source Han Code JP R"/>
@@ -270,6 +263,17 @@
       <color theme="1"/>
       <name val="Source Han Code JP H"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Grande Bold"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Lucida Grande Bold"/>
     </font>
   </fonts>
   <fills count="2">
@@ -301,25 +305,26 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="15" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -649,460 +654,407 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="35.33203125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.5" style="15" customWidth="1"/>
     <col min="3" max="3" width="12.5" style="1" customWidth="1"/>
     <col min="4" max="4" width="35.33203125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="19.5" style="1" customWidth="1"/>
+    <col min="5" max="5" width="19.5" style="15" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="13" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="15"/>
+      <c r="B1" s="9"/>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="15"/>
-      <c r="C2" s="8"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="8"/>
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
     </row>
     <row r="3" spans="1:5" ht="18" x14ac:dyDescent="0.3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="15" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="8"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="8"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
     </row>
     <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A4" s="8"/>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
+      <c r="A4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
     </row>
     <row r="5" spans="1:5" ht="16" x14ac:dyDescent="0.25">
-      <c r="A5" s="11" t="s">
+      <c r="A5" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="11" t="s">
+      <c r="B5" s="16"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="3"/>
+      <c r="E5" s="16"/>
     </row>
     <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="8"/>
-      <c r="D6" s="4" t="s">
+      <c r="C6" s="4"/>
+      <c r="D6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="5" t="s">
+      <c r="E6" s="10" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="8"/>
-      <c r="D7" s="8" t="s">
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="13" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8" t="s">
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="E8" s="9" t="s">
+      <c r="E8" s="13" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
+      <c r="A9" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="4" t="s">
+      <c r="C9" s="4"/>
+      <c r="D9" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A10" s="7"/>
-      <c r="B10" s="5"/>
-      <c r="C10" s="8"/>
-      <c r="D10" s="4" t="s">
+      <c r="A10" s="3"/>
+      <c r="B10" s="10"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="5" t="s">
+      <c r="E10" s="10" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="16" x14ac:dyDescent="0.25">
-      <c r="A11" s="11" t="s">
+      <c r="A11" s="6" t="s">
         <v>47</v>
       </c>
       <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="4"/>
+      <c r="D11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E11" s="5" t="s">
+      <c r="E11" s="10" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B12" s="5" t="s">
+      <c r="B12" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="8"/>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="4"/>
+      <c r="D12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E12" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A13" s="4" t="s">
+      <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B13" s="5" t="s">
+      <c r="B13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="8"/>
-      <c r="D13" s="8" t="s">
+      <c r="C13" s="4"/>
+      <c r="D13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="E13" s="8" t="s">
+      <c r="E13" s="15" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="A14" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="8"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="4"/>
     </row>
     <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B15" s="5" t="s">
+      <c r="B15" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="C15" s="8"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4"/>
     </row>
     <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B16" s="5" t="s">
+      <c r="B16" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="8"/>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="4" t="s">
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5" t="s">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C17" s="8"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A18" s="8" t="s">
+      <c r="C17" s="4"/>
+      <c r="D17" s="4"/>
+    </row>
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="B18" s="9" t="s">
+      <c r="B18" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A19" s="4" t="s">
+      <c r="C18" s="4"/>
+      <c r="D18" s="4"/>
+    </row>
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="5" t="s">
+      <c r="B19" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C19" s="8"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-    </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A20" s="8" t="s">
+      <c r="C19" s="4"/>
+      <c r="D19" s="4"/>
+    </row>
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A20" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="8"/>
-      <c r="D20" s="8"/>
-      <c r="E20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+      <c r="C20" s="4"/>
+      <c r="D20" s="4"/>
+    </row>
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A21" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C21" s="8"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+      <c r="C21" s="4"/>
+      <c r="D21" s="4"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A22" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="8"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A23" s="8" t="s">
+      <c r="C22" s="4"/>
+      <c r="D22" s="4"/>
+    </row>
+    <row r="23" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A23" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C23" s="8"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A24" s="8" t="s">
+      <c r="C23" s="4"/>
+      <c r="D23" s="4"/>
+    </row>
+    <row r="24" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C24" s="8"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="5"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" ht="16" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="C24" s="4"/>
+      <c r="D24" s="4"/>
+    </row>
+    <row r="25" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="10"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+    </row>
+    <row r="26" spans="1:4" ht="16" x14ac:dyDescent="0.25">
+      <c r="A26" s="7" t="s">
         <v>54</v>
       </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="8"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A27" s="4" t="s">
+      <c r="B26" s="14"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+    </row>
+    <row r="27" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="C27" s="8"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A28" s="4" t="s">
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+    </row>
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="B28" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="8"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-    </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C30" s="8"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-    </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C31" s="8"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C32" s="8"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C33" s="8"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C34" s="8"/>
-      <c r="D34" s="8"/>
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C35" s="8"/>
-      <c r="D35" s="8"/>
-      <c r="E35" s="8"/>
-    </row>
-    <row r="36" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="C36" s="8"/>
-      <c r="D36" s="8"/>
-      <c r="E36" s="8"/>
-    </row>
-    <row r="37" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A37" s="8"/>
-      <c r="B37" s="8"/>
-      <c r="C37" s="8"/>
-      <c r="D37" s="8"/>
-      <c r="E37" s="8"/>
-    </row>
-    <row r="38" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
-      <c r="D38" s="8"/>
-      <c r="E38" s="8"/>
-    </row>
-    <row r="39" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
-      <c r="D39" s="8"/>
-      <c r="E39" s="8"/>
-    </row>
-    <row r="40" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A40" s="8"/>
-      <c r="B40" s="8"/>
-      <c r="C40" s="8"/>
-      <c r="D40" s="8"/>
-      <c r="E40" s="8"/>
-    </row>
-    <row r="41" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A41" s="8"/>
-      <c r="B41" s="8"/>
-      <c r="C41" s="8"/>
-      <c r="D41" s="8"/>
-      <c r="E41" s="8"/>
-    </row>
-    <row r="42" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="8"/>
-      <c r="B42" s="8"/>
-      <c r="C42" s="8"/>
-      <c r="D42" s="8"/>
-      <c r="E42" s="8"/>
-    </row>
-    <row r="43" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="8"/>
-      <c r="B43" s="8"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="8"/>
-      <c r="E43" s="8"/>
-    </row>
-    <row r="44" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="8"/>
-      <c r="B44" s="8"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="8"/>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A45" s="8"/>
-      <c r="B45" s="8"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="8"/>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A46" s="8"/>
-      <c r="B46" s="8"/>
-      <c r="C46" s="8"/>
-      <c r="D46" s="8"/>
-      <c r="E46" s="8"/>
-    </row>
-    <row r="47" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A47" s="8"/>
-      <c r="B47" s="8"/>
-      <c r="C47" s="8"/>
-      <c r="D47" s="8"/>
-      <c r="E47" s="8"/>
-    </row>
-    <row r="48" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A48" s="8"/>
-      <c r="B48" s="8"/>
-      <c r="C48" s="8"/>
-      <c r="D48" s="8"/>
-      <c r="E48" s="8"/>
-    </row>
-    <row r="49" spans="1:5" ht="15" x14ac:dyDescent="0.25">
-      <c r="A49" s="8"/>
-      <c r="B49" s="8"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="8"/>
-      <c r="E49" s="8"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="11"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+    </row>
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+    </row>
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C31" s="4"/>
+      <c r="D31" s="4"/>
+    </row>
+    <row r="32" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C32" s="4"/>
+      <c r="D32" s="4"/>
+    </row>
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C33" s="4"/>
+      <c r="D33" s="4"/>
+    </row>
+    <row r="34" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C34" s="4"/>
+      <c r="D34" s="4"/>
+    </row>
+    <row r="35" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C35" s="4"/>
+      <c r="D35" s="4"/>
+    </row>
+    <row r="36" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="C36" s="4"/>
+      <c r="D36" s="4"/>
+    </row>
+    <row r="37" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A37" s="4"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="4"/>
+    </row>
+    <row r="38" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A38" s="4"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="4"/>
+    </row>
+    <row r="39" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A39" s="4"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="4"/>
+    </row>
+    <row r="40" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A40" s="4"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="4"/>
+    </row>
+    <row r="41" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A41" s="4"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="4"/>
+    </row>
+    <row r="42" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="4"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="4"/>
+    </row>
+    <row r="43" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A43" s="4"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="4"/>
+    </row>
+    <row r="44" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="4"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="4"/>
+    </row>
+    <row r="45" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A45" s="4"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="4"/>
+    </row>
+    <row r="46" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+    </row>
+    <row r="47" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A47" s="4"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+    </row>
+    <row r="48" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A48" s="4"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="4"/>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>